<commit_message>
Update appendix A (#190)
* Delete APPENDIX A - FedRAMP Tailored Security Controls Baseline.xlsx

* upload-fixed-appendixA
</commit_message>
<xml_diff>
--- a/static/APPENDIX A - FedRAMP Tailored Security Controls Baseline.xlsx
+++ b/static/APPENDIX A - FedRAMP Tailored Security Controls Baseline.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\OneDrive - Noblis, Inc\_FedRAMP\_CURRENT_PROJECTS\FedRAMP Tailored Revsions\2017-08-21 Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105" tabRatio="729" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9105" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="Key to LI-SaaS Baseline" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="329">
   <si>
     <t>SC-15</t>
   </si>
@@ -1115,9 +1115,6 @@
       <t>SaaS.
 NOTE: If the SaaS resides on a non-FedRAMP system, the CSP must treat all inherited controls as required.</t>
     </r>
-  </si>
-  <si>
-    <t>Controls FedRAMP determined are not required for Low Impact Cloud SaaS, and are independently assessed.</t>
   </si>
   <si>
     <r>
@@ -1244,6 +1241,12 @@
   </si>
   <si>
     <t>Document finalized for publication and use.</t>
+  </si>
+  <si>
+    <t>Minor correction to "Required" definition</t>
+  </si>
+  <si>
+    <t>Controls FedRAMP determined are required for Low Impact Cloud SaaS, and are independently assessed.</t>
   </si>
 </sst>
 </file>
@@ -1968,6 +1971,18 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2030,18 +2045,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2433,10 +2436,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E29"/>
+  <dimension ref="B1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2456,12 +2459,12 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -2472,12 +2475,12 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="62" t="s">
         <v>318</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
@@ -2495,70 +2498,70 @@
       <c r="B7" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="68"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="2:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="73" t="s">
         <v>278</v>
       </c>
-      <c r="D8" s="70"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="69" t="s">
-        <v>326</v>
-      </c>
-      <c r="D9" s="70"/>
+      <c r="C9" s="73" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" s="74"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C10" s="69" t="s">
-        <v>320</v>
-      </c>
-      <c r="D10" s="70"/>
+      <c r="C10" s="73" t="s">
+        <v>328</v>
+      </c>
+      <c r="D10" s="74"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="2:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="73" t="s">
         <v>314</v>
       </c>
-      <c r="D11" s="70"/>
+      <c r="D11" s="74"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:5" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="73" t="s">
         <v>319</v>
       </c>
-      <c r="D12" s="70"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="2:5" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="75" t="s">
         <v>315</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="76"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2568,32 +2571,32 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="63"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
     </row>
     <row r="16" spans="2:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="C17" s="59" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" s="63" t="s">
         <v>272</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="60"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="64"/>
     </row>
     <row r="18" spans="2:5" ht="48" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>273</v>
@@ -2614,12 +2617,12 @@
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="2:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="48" t="s">
@@ -2668,7 +2671,7 @@
         <v>41508</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D25" s="17">
         <v>3</v>
@@ -2678,28 +2681,42 @@
       </c>
     </row>
     <row r="26" spans="2:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="75"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="B26" s="54">
+        <v>41562</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" s="56">
+        <v>3.1</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="54"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
+    </row>
+    <row r="28" spans="2:5" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2752,13 +2769,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:89" s="35" customFormat="1" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>323</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
+      <c r="A1" s="77" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
@@ -8552,7 +8569,7 @@
   </sheetPr>
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -8567,13 +8584,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
-        <v>324</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="A1" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
     </row>
     <row r="2" spans="1:5" s="47" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -9086,7 +9103,7 @@
         <v>256</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>